<commit_message>
updated diagramme de gantt.xlsx
</commit_message>
<xml_diff>
--- a/documentation/diagramme de gantt.xlsx
+++ b/documentation/diagramme de gantt.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1F2758-1AFB-4B3B-ACEC-577932C86390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1737F4-A2CD-4F98-AC1A-09E5C4373254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -941,6 +941,15 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -948,47 +957,26 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
+    <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
     <cellStyle name="Date" xfId="10" xr:uid="{229918B6-DD13-4F5A-97B9-305F7E002AA3}"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Milliers" xfId="4" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Name" xfId="11" xr:uid="{B2D3C1EE-6B41-4801-AAFC-C2274E49E503}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pourcentage" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
     <cellStyle name="Project Start" xfId="9" xr:uid="{8EB8A09A-C31C-40A3-B2C1-9449520178B8}"/>
     <cellStyle name="Task" xfId="12" xr:uid="{6391D789-272B-4DD2-9BF3-2CDCF610FA41}"/>
-    <cellStyle name="Titre" xfId="5" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Titre 1" xfId="6" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Titre 2" xfId="7" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Titre 3" xfId="8" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1006,6 +994,18 @@
           <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <border>
@@ -1528,25 +1528,25 @@
   </sheetPr>
   <dimension ref="A1:CG34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.69140625" style="58" customWidth="1"/>
-    <col min="2" max="2" width="48.53515625" customWidth="1"/>
-    <col min="3" max="3" width="30.69140625" customWidth="1"/>
-    <col min="4" max="4" width="10.69140625" customWidth="1"/>
-    <col min="5" max="5" width="10.4609375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.4609375" customWidth="1"/>
-    <col min="7" max="7" width="2.69140625" customWidth="1"/>
-    <col min="8" max="8" width="6.07421875" hidden="1" customWidth="1"/>
-    <col min="9" max="85" width="2.53515625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="58" customWidth="1"/>
+    <col min="2" max="2" width="48.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" hidden="1" customWidth="1"/>
+    <col min="9" max="85" width="2.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="59" t="s">
         <v>32</v>
       </c>
@@ -1560,470 +1560,470 @@
       <c r="H1" s="2"/>
       <c r="I1" s="14"/>
     </row>
-    <row r="2" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="58" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="64"/>
       <c r="I2" s="61"/>
     </row>
-    <row r="3" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="58" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="65"/>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="91"/>
+      <c r="D3" s="94"/>
       <c r="E3" s="96">
         <f>DATE(2021,12,1)</f>
         <v>44531</v>
       </c>
       <c r="F3" s="96"/>
     </row>
-    <row r="4" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="91"/>
+      <c r="D4" s="94"/>
       <c r="E4" s="7">
-        <v>10</v>
-      </c>
-      <c r="I4" s="93">
+        <v>1</v>
+      </c>
+      <c r="I4" s="90">
         <f>I5</f>
+        <v>44529</v>
+      </c>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="90">
+        <f>P5</f>
+        <v>44536</v>
+      </c>
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="92"/>
+      <c r="W4" s="90">
+        <f>W5</f>
+        <v>44543</v>
+      </c>
+      <c r="X4" s="91"/>
+      <c r="Y4" s="91"/>
+      <c r="Z4" s="91"/>
+      <c r="AA4" s="91"/>
+      <c r="AB4" s="91"/>
+      <c r="AC4" s="92"/>
+      <c r="AD4" s="90">
+        <f>AD5</f>
+        <v>44550</v>
+      </c>
+      <c r="AE4" s="91"/>
+      <c r="AF4" s="91"/>
+      <c r="AG4" s="91"/>
+      <c r="AH4" s="91"/>
+      <c r="AI4" s="91"/>
+      <c r="AJ4" s="92"/>
+      <c r="AK4" s="90">
+        <f>AK5</f>
+        <v>44557</v>
+      </c>
+      <c r="AL4" s="91"/>
+      <c r="AM4" s="91"/>
+      <c r="AN4" s="91"/>
+      <c r="AO4" s="91"/>
+      <c r="AP4" s="91"/>
+      <c r="AQ4" s="92"/>
+      <c r="AR4" s="90">
+        <f>AR5</f>
+        <v>44564</v>
+      </c>
+      <c r="AS4" s="91"/>
+      <c r="AT4" s="91"/>
+      <c r="AU4" s="91"/>
+      <c r="AV4" s="91"/>
+      <c r="AW4" s="91"/>
+      <c r="AX4" s="92"/>
+      <c r="AY4" s="90">
+        <f>AY5</f>
+        <v>44571</v>
+      </c>
+      <c r="AZ4" s="91"/>
+      <c r="BA4" s="91"/>
+      <c r="BB4" s="91"/>
+      <c r="BC4" s="91"/>
+      <c r="BD4" s="91"/>
+      <c r="BE4" s="92"/>
+      <c r="BF4" s="90">
+        <f>BF5</f>
+        <v>44578</v>
+      </c>
+      <c r="BG4" s="91"/>
+      <c r="BH4" s="91"/>
+      <c r="BI4" s="91"/>
+      <c r="BJ4" s="91"/>
+      <c r="BK4" s="91"/>
+      <c r="BL4" s="92"/>
+      <c r="BM4" s="90">
+        <f>BM5</f>
+        <v>44585</v>
+      </c>
+      <c r="BN4" s="91"/>
+      <c r="BO4" s="91"/>
+      <c r="BP4" s="91"/>
+      <c r="BQ4" s="91"/>
+      <c r="BR4" s="91"/>
+      <c r="BS4" s="92"/>
+      <c r="BT4" s="90">
+        <f>BT5</f>
         <v>44592</v>
       </c>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="94"/>
-      <c r="O4" s="95"/>
-      <c r="P4" s="93">
-        <f>P5</f>
+      <c r="BU4" s="91"/>
+      <c r="BV4" s="91"/>
+      <c r="BW4" s="91"/>
+      <c r="BX4" s="91"/>
+      <c r="BY4" s="91"/>
+      <c r="BZ4" s="92"/>
+      <c r="CA4" s="90">
+        <f>CA5</f>
         <v>44599</v>
       </c>
-      <c r="Q4" s="94"/>
-      <c r="R4" s="94"/>
-      <c r="S4" s="94"/>
-      <c r="T4" s="94"/>
-      <c r="U4" s="94"/>
-      <c r="V4" s="95"/>
-      <c r="W4" s="93">
-        <f>W5</f>
-        <v>44606</v>
-      </c>
-      <c r="X4" s="94"/>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="94"/>
-      <c r="AA4" s="94"/>
-      <c r="AB4" s="94"/>
-      <c r="AC4" s="95"/>
-      <c r="AD4" s="93">
-        <f>AD5</f>
-        <v>44613</v>
-      </c>
-      <c r="AE4" s="94"/>
-      <c r="AF4" s="94"/>
-      <c r="AG4" s="94"/>
-      <c r="AH4" s="94"/>
-      <c r="AI4" s="94"/>
-      <c r="AJ4" s="95"/>
-      <c r="AK4" s="93">
-        <f>AK5</f>
-        <v>44620</v>
-      </c>
-      <c r="AL4" s="94"/>
-      <c r="AM4" s="94"/>
-      <c r="AN4" s="94"/>
-      <c r="AO4" s="94"/>
-      <c r="AP4" s="94"/>
-      <c r="AQ4" s="95"/>
-      <c r="AR4" s="93">
-        <f>AR5</f>
-        <v>44627</v>
-      </c>
-      <c r="AS4" s="94"/>
-      <c r="AT4" s="94"/>
-      <c r="AU4" s="94"/>
-      <c r="AV4" s="94"/>
-      <c r="AW4" s="94"/>
-      <c r="AX4" s="95"/>
-      <c r="AY4" s="93">
-        <f>AY5</f>
-        <v>44634</v>
-      </c>
-      <c r="AZ4" s="94"/>
-      <c r="BA4" s="94"/>
-      <c r="BB4" s="94"/>
-      <c r="BC4" s="94"/>
-      <c r="BD4" s="94"/>
-      <c r="BE4" s="95"/>
-      <c r="BF4" s="93">
-        <f>BF5</f>
-        <v>44641</v>
-      </c>
-      <c r="BG4" s="94"/>
-      <c r="BH4" s="94"/>
-      <c r="BI4" s="94"/>
-      <c r="BJ4" s="94"/>
-      <c r="BK4" s="94"/>
-      <c r="BL4" s="95"/>
-      <c r="BM4" s="93">
-        <f>BM5</f>
-        <v>44648</v>
-      </c>
-      <c r="BN4" s="94"/>
-      <c r="BO4" s="94"/>
-      <c r="BP4" s="94"/>
-      <c r="BQ4" s="94"/>
-      <c r="BR4" s="94"/>
-      <c r="BS4" s="95"/>
-      <c r="BT4" s="93">
-        <f>BT5</f>
-        <v>44655</v>
-      </c>
-      <c r="BU4" s="94"/>
-      <c r="BV4" s="94"/>
-      <c r="BW4" s="94"/>
-      <c r="BX4" s="94"/>
-      <c r="BY4" s="94"/>
-      <c r="BZ4" s="95"/>
-      <c r="CA4" s="93">
-        <f>CA5</f>
-        <v>44662</v>
-      </c>
-      <c r="CB4" s="94"/>
-      <c r="CC4" s="94"/>
-      <c r="CD4" s="94"/>
-      <c r="CE4" s="94"/>
-      <c r="CF4" s="94"/>
-      <c r="CG4" s="95"/>
+      <c r="CB4" s="91"/>
+      <c r="CC4" s="91"/>
+      <c r="CD4" s="91"/>
+      <c r="CE4" s="91"/>
+      <c r="CF4" s="91"/>
+      <c r="CG4" s="92"/>
     </row>
-    <row r="5" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:85" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>44592</v>
+        <v>44529</v>
       </c>
       <c r="J5" s="10">
         <f>I5+1</f>
-        <v>44593</v>
+        <v>44530</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" si="0">J5+1</f>
-        <v>44594</v>
+        <v>44531</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" si="0"/>
-        <v>44595</v>
+        <v>44532</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" si="0"/>
-        <v>44596</v>
+        <v>44533</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" si="0"/>
-        <v>44597</v>
+        <v>44534</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" si="0"/>
-        <v>44598</v>
+        <v>44535</v>
       </c>
       <c r="P5" s="11">
         <f>O5+1</f>
-        <v>44599</v>
+        <v>44536</v>
       </c>
       <c r="Q5" s="10">
         <f>P5+1</f>
-        <v>44600</v>
+        <v>44537</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" si="0"/>
-        <v>44601</v>
+        <v>44538</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" si="0"/>
-        <v>44602</v>
+        <v>44539</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" si="0"/>
-        <v>44603</v>
+        <v>44540</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" si="0"/>
-        <v>44604</v>
+        <v>44541</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" si="0"/>
-        <v>44605</v>
+        <v>44542</v>
       </c>
       <c r="W5" s="11">
         <f>V5+1</f>
-        <v>44606</v>
+        <v>44543</v>
       </c>
       <c r="X5" s="10">
         <f>W5+1</f>
-        <v>44607</v>
+        <v>44544</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" si="0"/>
-        <v>44608</v>
+        <v>44545</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" si="0"/>
-        <v>44609</v>
+        <v>44546</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" si="0"/>
-        <v>44610</v>
+        <v>44547</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" si="0"/>
-        <v>44611</v>
+        <v>44548</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" si="0"/>
-        <v>44612</v>
+        <v>44549</v>
       </c>
       <c r="AD5" s="11">
         <f>AC5+1</f>
-        <v>44613</v>
+        <v>44550</v>
       </c>
       <c r="AE5" s="10">
         <f>AD5+1</f>
-        <v>44614</v>
+        <v>44551</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" si="0"/>
-        <v>44615</v>
+        <v>44552</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" si="0"/>
-        <v>44616</v>
+        <v>44553</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" si="0"/>
-        <v>44617</v>
+        <v>44554</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" si="0"/>
-        <v>44618</v>
+        <v>44555</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" si="0"/>
-        <v>44619</v>
+        <v>44556</v>
       </c>
       <c r="AK5" s="11">
         <f>AJ5+1</f>
-        <v>44620</v>
+        <v>44557</v>
       </c>
       <c r="AL5" s="10">
         <f>AK5+1</f>
-        <v>44621</v>
+        <v>44558</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" si="0"/>
-        <v>44622</v>
+        <v>44559</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" si="0"/>
-        <v>44623</v>
+        <v>44560</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" si="0"/>
-        <v>44624</v>
+        <v>44561</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" si="0"/>
-        <v>44625</v>
+        <v>44562</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" si="0"/>
-        <v>44626</v>
+        <v>44563</v>
       </c>
       <c r="AR5" s="11">
         <f>AQ5+1</f>
-        <v>44627</v>
+        <v>44564</v>
       </c>
       <c r="AS5" s="10">
         <f>AR5+1</f>
-        <v>44628</v>
+        <v>44565</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" si="0"/>
-        <v>44629</v>
+        <v>44566</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" si="0"/>
-        <v>44630</v>
+        <v>44567</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" si="0"/>
-        <v>44631</v>
+        <v>44568</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" si="0"/>
-        <v>44632</v>
+        <v>44569</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" si="0"/>
-        <v>44633</v>
+        <v>44570</v>
       </c>
       <c r="AY5" s="11">
         <f>AX5+1</f>
-        <v>44634</v>
+        <v>44571</v>
       </c>
       <c r="AZ5" s="10">
         <f>AY5+1</f>
-        <v>44635</v>
+        <v>44572</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
-        <v>44636</v>
+        <v>44573</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" si="1"/>
-        <v>44637</v>
+        <v>44574</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" si="1"/>
-        <v>44638</v>
+        <v>44575</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" si="1"/>
-        <v>44639</v>
+        <v>44576</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" si="1"/>
-        <v>44640</v>
+        <v>44577</v>
       </c>
       <c r="BF5" s="11">
         <f>BE5+1</f>
-        <v>44641</v>
+        <v>44578</v>
       </c>
       <c r="BG5" s="10">
         <f>BF5+1</f>
-        <v>44642</v>
+        <v>44579</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
-        <v>44643</v>
+        <v>44580</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" si="2"/>
-        <v>44644</v>
+        <v>44581</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" si="2"/>
-        <v>44645</v>
+        <v>44582</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" si="2"/>
-        <v>44646</v>
+        <v>44583</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" si="2"/>
-        <v>44647</v>
+        <v>44584</v>
       </c>
       <c r="BM5" s="11">
         <f t="shared" ref="BM5:CG5" si="3">BL5+1</f>
-        <v>44648</v>
+        <v>44585</v>
       </c>
       <c r="BN5" s="10">
         <f t="shared" si="3"/>
-        <v>44649</v>
+        <v>44586</v>
       </c>
       <c r="BO5" s="10">
         <f t="shared" si="3"/>
-        <v>44650</v>
+        <v>44587</v>
       </c>
       <c r="BP5" s="10">
         <f t="shared" si="3"/>
-        <v>44651</v>
+        <v>44588</v>
       </c>
       <c r="BQ5" s="10">
         <f t="shared" si="3"/>
-        <v>44652</v>
+        <v>44589</v>
       </c>
       <c r="BR5" s="10">
         <f t="shared" si="3"/>
-        <v>44653</v>
+        <v>44590</v>
       </c>
       <c r="BS5" s="12">
         <f t="shared" si="3"/>
-        <v>44654</v>
+        <v>44591</v>
       </c>
       <c r="BT5" s="11">
         <f t="shared" si="3"/>
-        <v>44655</v>
+        <v>44592</v>
       </c>
       <c r="BU5" s="10">
         <f t="shared" si="3"/>
-        <v>44656</v>
+        <v>44593</v>
       </c>
       <c r="BV5" s="10">
         <f t="shared" si="3"/>
-        <v>44657</v>
+        <v>44594</v>
       </c>
       <c r="BW5" s="10">
         <f t="shared" si="3"/>
-        <v>44658</v>
+        <v>44595</v>
       </c>
       <c r="BX5" s="10">
         <f t="shared" si="3"/>
-        <v>44659</v>
+        <v>44596</v>
       </c>
       <c r="BY5" s="10">
         <f t="shared" si="3"/>
-        <v>44660</v>
+        <v>44597</v>
       </c>
       <c r="BZ5" s="12">
         <f t="shared" si="3"/>
-        <v>44661</v>
+        <v>44598</v>
       </c>
       <c r="CA5" s="11">
         <f t="shared" si="3"/>
-        <v>44662</v>
+        <v>44599</v>
       </c>
       <c r="CB5" s="10">
         <f t="shared" si="3"/>
-        <v>44663</v>
+        <v>44600</v>
       </c>
       <c r="CC5" s="10">
         <f t="shared" si="3"/>
-        <v>44664</v>
+        <v>44601</v>
       </c>
       <c r="CD5" s="10">
         <f t="shared" si="3"/>
-        <v>44665</v>
+        <v>44602</v>
       </c>
       <c r="CE5" s="10">
         <f t="shared" si="3"/>
-        <v>44666</v>
+        <v>44603</v>
       </c>
       <c r="CF5" s="10">
         <f t="shared" si="3"/>
-        <v>44667</v>
+        <v>44604</v>
       </c>
       <c r="CG5" s="12">
         <f t="shared" si="3"/>
-        <v>44668</v>
+        <v>44605</v>
       </c>
     </row>
-    <row r="6" spans="1:85" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:85" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="59" t="s">
         <v>36</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:85" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:85" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="58" t="s">
         <v>31</v>
       </c>
@@ -2443,7 +2443,7 @@
       <c r="CF7" s="44"/>
       <c r="CG7" s="44"/>
     </row>
-    <row r="8" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="59" t="s">
         <v>37</v>
       </c>
@@ -2537,7 +2537,7 @@
       <c r="CF8" s="44"/>
       <c r="CG8" s="44"/>
     </row>
-    <row r="9" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="59" t="s">
         <v>38</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>62</v>
       </c>
       <c r="D9" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="66">
         <f>Project_Start</f>
@@ -2641,7 +2641,7 @@
       <c r="CF9" s="44"/>
       <c r="CG9" s="44"/>
     </row>
-    <row r="10" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="59" t="s">
         <v>39</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>59</v>
       </c>
       <c r="D10" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="66">
         <f>F9+1</f>
@@ -2745,7 +2745,7 @@
       <c r="CF10" s="44"/>
       <c r="CG10" s="44"/>
     </row>
-    <row r="11" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="58"/>
       <c r="B11" s="72" t="s">
         <v>46</v>
@@ -2754,7 +2754,7 @@
         <v>59</v>
       </c>
       <c r="D11" s="22">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E11" s="66">
         <f>F10+1</f>
@@ -2847,7 +2847,7 @@
       <c r="CF11" s="44"/>
       <c r="CG11" s="44"/>
     </row>
-    <row r="12" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="58"/>
       <c r="B12" s="72" t="s">
         <v>48</v>
@@ -2856,7 +2856,7 @@
         <v>49</v>
       </c>
       <c r="D12" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="66">
         <f>F9+1</f>
@@ -2949,7 +2949,7 @@
       <c r="CF12" s="44"/>
       <c r="CG12" s="44"/>
     </row>
-    <row r="13" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="58"/>
       <c r="B13" s="72" t="s">
         <v>47</v>
@@ -2965,7 +2965,7 @@
         <v>44567</v>
       </c>
       <c r="F13" s="66">
-        <f t="shared" ref="F12:F13" si="9">E13+6</f>
+        <f t="shared" ref="F13" si="9">E13+6</f>
         <v>44573</v>
       </c>
       <c r="G13" s="17"/>
@@ -3051,7 +3051,7 @@
       <c r="CF13" s="44"/>
       <c r="CG13" s="44"/>
     </row>
-    <row r="14" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="59" t="s">
         <v>40</v>
       </c>
@@ -3145,7 +3145,7 @@
       <c r="CF14" s="44"/>
       <c r="CG14" s="44"/>
     </row>
-    <row r="15" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="59"/>
       <c r="B15" s="83" t="s">
         <v>41</v>
@@ -3247,7 +3247,7 @@
       <c r="CF15" s="44"/>
       <c r="CG15" s="44"/>
     </row>
-    <row r="16" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="58"/>
       <c r="B16" s="83" t="s">
         <v>43</v>
@@ -3349,7 +3349,7 @@
       <c r="CF16" s="44"/>
       <c r="CG16" s="44"/>
     </row>
-    <row r="17" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="58"/>
       <c r="B17" s="83" t="s">
         <v>44</v>
@@ -3451,7 +3451,7 @@
       <c r="CF17" s="44"/>
       <c r="CG17" s="44"/>
     </row>
-    <row r="18" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="58"/>
       <c r="B18" s="83" t="s">
         <v>42</v>
@@ -3460,7 +3460,7 @@
         <v>49</v>
       </c>
       <c r="D18" s="27">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E18" s="67">
         <f>F17+1</f>
@@ -3553,7 +3553,7 @@
       <c r="CF18" s="44"/>
       <c r="CG18" s="44"/>
     </row>
-    <row r="19" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="58" t="s">
         <v>28</v>
       </c>
@@ -3647,7 +3647,7 @@
       <c r="CF19" s="44"/>
       <c r="CG19" s="44"/>
     </row>
-    <row r="20" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="58"/>
       <c r="B20" s="86" t="s">
         <v>53</v>
@@ -3749,7 +3749,7 @@
       <c r="CF20" s="44"/>
       <c r="CG20" s="44"/>
     </row>
-    <row r="21" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="58"/>
       <c r="B21" s="87" t="s">
         <v>55</v>
@@ -3851,7 +3851,7 @@
       <c r="CF21" s="44"/>
       <c r="CG21" s="44"/>
     </row>
-    <row r="22" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="58"/>
       <c r="B22" s="86" t="s">
         <v>54</v>
@@ -3953,7 +3953,7 @@
       <c r="CF22" s="44"/>
       <c r="CG22" s="44"/>
     </row>
-    <row r="23" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="58"/>
       <c r="B23" s="84" t="s">
         <v>52</v>
@@ -4055,7 +4055,7 @@
       <c r="CF23" s="44"/>
       <c r="CG23" s="44"/>
     </row>
-    <row r="24" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="58" t="s">
         <v>28</v>
       </c>
@@ -4149,7 +4149,7 @@
       <c r="CF24" s="44"/>
       <c r="CG24" s="44"/>
     </row>
-    <row r="25" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="58"/>
       <c r="B25" s="88" t="s">
         <v>61</v>
@@ -4251,7 +4251,7 @@
       <c r="CF25" s="44"/>
       <c r="CG25" s="44"/>
     </row>
-    <row r="26" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="58"/>
       <c r="B26" s="88" t="s">
         <v>63</v>
@@ -4353,7 +4353,7 @@
       <c r="CF26" s="44"/>
       <c r="CG26" s="44"/>
     </row>
-    <row r="27" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="58"/>
       <c r="B27" s="89" t="s">
         <v>64</v>
@@ -4455,7 +4455,7 @@
       <c r="CF27" s="44"/>
       <c r="CG27" s="44"/>
     </row>
-    <row r="28" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="58"/>
       <c r="B28" s="80" t="s">
         <v>0</v>
@@ -4551,7 +4551,7 @@
       <c r="CF28" s="44"/>
       <c r="CG28" s="44"/>
     </row>
-    <row r="29" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="58"/>
       <c r="B29" s="80" t="s">
         <v>1</v>
@@ -4647,7 +4647,7 @@
       <c r="CF29" s="44"/>
       <c r="CG29" s="44"/>
     </row>
-    <row r="30" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="58" t="s">
         <v>30</v>
       </c>
@@ -4739,7 +4739,7 @@
       <c r="CF30" s="44"/>
       <c r="CG30" s="44"/>
     </row>
-    <row r="31" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:85" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="59" t="s">
         <v>29</v>
       </c>
@@ -4833,23 +4833,18 @@
       <c r="CF31" s="46"/>
       <c r="CG31" s="46"/>
     </row>
-    <row r="32" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C33" s="14"/>
       <c r="F33" s="60"/>
     </row>
-    <row r="34" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B5:G5"/>
@@ -4860,6 +4855,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
   </mergeCells>
   <conditionalFormatting sqref="D24:D31 D7:D22">
     <cfRule type="dataBar" priority="15">
@@ -4876,15 +4876,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:CG31">
-    <cfRule type="expression" dxfId="0" priority="34">
+    <cfRule type="expression" dxfId="2" priority="34">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:CG31">
-    <cfRule type="expression" dxfId="2" priority="28">
+    <cfRule type="expression" dxfId="1" priority="28">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="29" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4958,86 +4958,86 @@
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.07421875" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="87.07421875" style="48" customWidth="1"/>
-    <col min="2" max="16384" width="9.07421875" style="2"/>
+    <col min="1" max="1" width="87.109375" style="48" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:2" s="50" customFormat="1" ht="15.9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" s="50" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="49"/>
     </row>
-    <row r="3" spans="1:2" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="55" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="55"/>
     </row>
-    <row r="4" spans="1:2" s="51" customFormat="1" ht="26.15" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:2" s="51" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" s="52" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="53" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="52" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="48" customFormat="1" ht="204.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" s="48" customFormat="1" ht="204.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="57" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="51" customFormat="1" ht="26.15" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:2" s="51" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" s="52" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="58.3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="53" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="48" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" s="48" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="56" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="51" customFormat="1" ht="26.15" x14ac:dyDescent="0.7">
+    <row r="11" spans="1:2" s="51" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A11" s="52" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="29.15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="53" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="48" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" s="48" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="56" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="51" customFormat="1" ht="26.15" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:2" s="51" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A14" s="52" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="53" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="53" t="s">
         <v>18</v>
       </c>
@@ -5056,6 +5056,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010026BC1444C3903B40AEE050BD15B05899" ma:contentTypeVersion="7" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="8a500c66f87445244be80e92d31b92b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="27b1b7b1-91e2-4143-8608-e99651b31e6b" xmlns:ns4="69049c1a-4801-419a-8bbf-52269bce4c2d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="18438fbda9c9406c4237cfb524b73c28" ns3:_="" ns4:_="">
     <xsd:import namespace="27b1b7b1-91e2-4143-8608-e99651b31e6b"/>
@@ -5240,22 +5255,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28F7E4E8-3BEC-4BF7-A6DB-9E941E22FF6B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="69049c1a-4801-419a-8bbf-52269bce4c2d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="27b1b7b1-91e2-4143-8608-e99651b31e6b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB045FA5-BA1B-4CE7-B3D8-13C9905AFB53}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17F00616-6607-4E3F-AC14-5FD1093F399D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5272,29 +5297,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB045FA5-BA1B-4CE7-B3D8-13C9905AFB53}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28F7E4E8-3BEC-4BF7-A6DB-9E941E22FF6B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="69049c1a-4801-419a-8bbf-52269bce4c2d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="27b1b7b1-91e2-4143-8608-e99651b31e6b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>